<commit_message>
entity info reflects all stats
</commit_message>
<xml_diff>
--- a/reference/combat_modelling.xlsx
+++ b/reference/combat_modelling.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Documents\NotQuiteParadise\reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53670E5-638C-4446-99E6-EFE674D963C9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE8B4C3-B416-4479-916C-9620EF8B4369}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36450" yWindow="0" windowWidth="15150" windowHeight="21000" activeTab="2" xr2:uid="{B61F704B-B289-4DB0-8A42-128F7E4E2B4C}"/>
   </bookViews>
@@ -839,21 +839,6 @@
   </cellStyles>
   <dxfs count="47">
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Bahnschrift Light SemiCondensed"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1301,6 +1286,21 @@
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Bahnschrift Light SemiCondensed"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1541,11 +1541,11 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{56842182-A38F-472C-8F28-74F940CA139A}" name="entity_primary_stats" displayName="entity_primary_stats" ref="B4:H9" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00F24B6A-A907-4E37-8082-FC7DA03CD0E4}" name="Name" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{00F24B6A-A907-4E37-8082-FC7DA03CD0E4}" name="Name" dataDxfId="32">
       <calculatedColumnFormula>Lists!B2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{B612A34B-677F-4CF3-9DB1-A4DEF7A0ECC0}" name="Purpose" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{D00B2AAA-E32A-4AED-B6E4-C6D71C6713CC}" name="Influences" dataDxfId="31">
+    <tableColumn id="2" xr3:uid="{B612A34B-677F-4CF3-9DB1-A4DEF7A0ECC0}" name="Purpose" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{D00B2AAA-E32A-4AED-B6E4-C6D71C6713CC}" name="Influences" dataDxfId="30">
       <calculatedColumnFormula>IF(OR($N$5=C5,$P$5=C5,$R$5=C5),$K$5 &amp; ", ","") &amp;
 IF(OR($N$6=C5,$P$6=C5,$R$6=C5),$K$6 &amp; ", ","") &amp;
 IF(OR($N$7=C5,$P$7=C5,$R$7=C5),$K$7 &amp; ", ","") &amp;
@@ -1558,31 +1558,31 @@
 IF(OR($N$14=C5,$P$14=C5,$R$14=C5),$K$14 &amp; ", ","") &amp;
 IF(OR($N$15=C5,$P$15=C5,$R$15=C5),$K$15 &amp; ", ","")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{E4038DD6-1CD5-43C6-9217-100476CEC204}" name="# influenced stats" dataDxfId="30">
+    <tableColumn id="4" xr3:uid="{E4038DD6-1CD5-43C6-9217-100476CEC204}" name="# influenced stats" dataDxfId="29">
       <calculatedColumnFormula>LEN(D5)-LEN(SUBSTITUTE(D5,",",""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{175CFB49-E265-4916-B0C4-D5DEA5BEBF51}" name="Stat value" dataDxfId="29">
+    <tableColumn id="7" xr3:uid="{175CFB49-E265-4916-B0C4-D5DEA5BEBF51}" name="Stat value" dataDxfId="28">
       <calculatedColumnFormula>SUMIF(entity_derived_stats[Derived from (1)],entity_primary_stats[[#This Row],[Name]],entity_derived_stats[Amount Derived (1)]) + SUMIF(entity_derived_stats[Derived from (2)],entity_primary_stats[[#This Row],[Name]],entity_derived_stats[Amount Derived (2)]) + SUMIF(entity_derived_stats[Derived from (3)],entity_primary_stats[[#This Row],[Name]],entity_derived_stats[Amount Derived (3)])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{C9B7ABCA-BC18-4059-B614-A6254871E453}" name="min # " dataDxfId="28"/>
-    <tableColumn id="6" xr3:uid="{77EC5584-7C71-434B-8C87-E752B3CA1F16}" name="max #" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{C9B7ABCA-BC18-4059-B614-A6254871E453}" name="min # " dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{77EC5584-7C71-434B-8C87-E752B3CA1F16}" name="max #" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F4B1EC6D-90B4-4431-8769-8725ACDB1262}" name="adult" displayName="adult" ref="J18:P20" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F4B1EC6D-90B4-4431-8769-8725ACDB1262}" name="adult" displayName="adult" ref="J18:P20" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{C498C6EC-EDCF-46B5-AC54-19697D44ACEE}" name="Name" dataDxfId="24">
+    <tableColumn id="1" xr3:uid="{C498C6EC-EDCF-46B5-AC54-19697D44ACEE}" name="Name" dataDxfId="23">
       <calculatedColumnFormula>Lists!F2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{173660BE-87D9-47FB-AA17-824F2720DA45}" name="Damage" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{14AD948D-BA0F-46D8-90E7-33C50DEE188A}" name="Accuracy" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{665079BF-14DC-4613-BA06-762971C6C47E}" name="Speed" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{47CFB954-5875-48DC-A786-5961B7D5B694}" name="Statuses" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{A39EAF1B-106D-4B64-9FE8-19283A107000}" name="Health" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{CC6A1BE2-5E8D-44B4-B68F-A740FC943358}" name="Total value" dataDxfId="18">
+    <tableColumn id="2" xr3:uid="{173660BE-87D9-47FB-AA17-824F2720DA45}" name="Damage" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{14AD948D-BA0F-46D8-90E7-33C50DEE188A}" name="Accuracy" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{665079BF-14DC-4613-BA06-762971C6C47E}" name="Speed" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{47CFB954-5875-48DC-A786-5961B7D5B694}" name="Statuses" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{A39EAF1B-106D-4B64-9FE8-19283A107000}" name="Health" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{CC6A1BE2-5E8D-44B4-B68F-A740FC943358}" name="Total value" dataDxfId="17">
       <calculatedColumnFormula>SUM(K19:O19)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1591,17 +1591,17 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DCB3CFA5-EDF9-4FEE-AC07-3B1486B62A80}" name="youth" displayName="youth" ref="B18:H20" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DCB3CFA5-EDF9-4FEE-AC07-3B1486B62A80}" name="youth" displayName="youth" ref="B18:H20" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{D75C2AFC-B2E2-4AD9-8D70-0092B38CAEBC}" name="Name" dataDxfId="15">
+    <tableColumn id="1" xr3:uid="{D75C2AFC-B2E2-4AD9-8D70-0092B38CAEBC}" name="Name" dataDxfId="14">
       <calculatedColumnFormula>Lists!D2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{3DFCE0EF-9561-447F-98CC-14C2AE7D7D94}" name="Damage" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{FE008038-ABB8-485E-9AB4-637C767011CA}" name="Accuracy" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{B48D67B2-B0DA-4E10-A588-E0E1BF2C9EE6}" name="Speed" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{45850A44-F014-4245-A354-C10DBFFC05EC}" name="Statuses" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{8D878A50-BA27-475A-BB61-3A54095090E4}" name="Health" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{CF1F4B93-9B1A-4429-AF43-D4CC73A31715}" name="Total value" dataDxfId="9">
+    <tableColumn id="2" xr3:uid="{3DFCE0EF-9561-447F-98CC-14C2AE7D7D94}" name="Damage" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{FE008038-ABB8-485E-9AB4-637C767011CA}" name="Accuracy" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{B48D67B2-B0DA-4E10-A588-E0E1BF2C9EE6}" name="Speed" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{45850A44-F014-4245-A354-C10DBFFC05EC}" name="Statuses" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{8D878A50-BA27-475A-BB61-3A54095090E4}" name="Health" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{CF1F4B93-9B1A-4429-AF43-D4CC73A31715}" name="Total value" dataDxfId="8">
       <calculatedColumnFormula>SUM(C19:G19)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1610,18 +1610,18 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{27A7BA62-89F1-47C8-BA1A-ACF34F294D38}" name="attack_skills" displayName="attack_skills" ref="B3:I5" totalsRowShown="0" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{27A7BA62-89F1-47C8-BA1A-ACF34F294D38}" name="attack_skills" displayName="attack_skills" ref="B3:I5" totalsRowShown="0" headerRowDxfId="7">
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{EB8E6709-1E4E-4270-AE23-0136B1CFFBB6}" name="Name">
       <calculatedColumnFormula>Lists!H2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{6CA35C9E-7272-4A55-A800-22AC2D20488E}" name="Base accuracy" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{AE37A56D-22F9-44A2-881D-6FEBE14B6684}" name="Accuracy type" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{79B30171-9C13-48D7-AEBC-E01824C15451}" name="Base damage" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{4AAF5594-E1B5-43C2-B0A6-BFE29D5199AE}" name="Damage type" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{F5C0387D-6960-4820-B8CE-85043E6F937C}" name="Cost" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{12DC5BF9-4E77-4D3F-A624-A73E0DADEF28}" name="Status Applied" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{92E43F99-EA94-459D-9EC5-23B0223BE593}" name="Status Length" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{6CA35C9E-7272-4A55-A800-22AC2D20488E}" name="Base accuracy" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{AE37A56D-22F9-44A2-881D-6FEBE14B6684}" name="Accuracy type" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{79B30171-9C13-48D7-AEBC-E01824C15451}" name="Base damage" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{4AAF5594-E1B5-43C2-B0A6-BFE29D5199AE}" name="Damage type" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{F5C0387D-6960-4820-B8CE-85043E6F937C}" name="Cost" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{12DC5BF9-4E77-4D3F-A624-A73E0DADEF28}" name="Status Applied" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{92E43F99-EA94-459D-9EC5-23B0223BE593}" name="Status Length" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2168,7 +2168,7 @@
   <dimension ref="B2:S25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
damage uses new stats
</commit_message>
<xml_diff>
--- a/reference/combat_modelling.xlsx
+++ b/reference/combat_modelling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Documents\NotQuiteParadise\reference\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE8B4C3-B416-4479-916C-9620EF8B4369}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED43347-BEAA-45B6-AD77-A822C9A898D7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36450" yWindow="0" windowWidth="15150" windowHeight="21000" activeTab="2" xr2:uid="{B61F704B-B289-4DB0-8A42-128F7E4E2B4C}"/>
+    <workbookView xWindow="36450" yWindow="0" windowWidth="15150" windowHeight="21000" activeTab="4" xr2:uid="{B61F704B-B289-4DB0-8A42-128F7E4E2B4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Reference_Data" sheetId="5" r:id="rId1"/>
@@ -2167,7 +2167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131F03A5-DDF5-4590-8C79-0FDF3BA926D3}">
   <dimension ref="B2:S25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
@@ -3102,7 +3102,7 @@
   <dimension ref="B1:I5"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3219,8 +3219,8 @@
   </sheetPr>
   <dimension ref="B1:X30"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4161,7 +4161,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="15">
     <mergeCell ref="T3:U3"/>
     <mergeCell ref="N2:X2"/>

</xml_diff>